<commit_message>
Updated sources and modified Table 3
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOC5670\Assignments\Homework01\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOC5670\Assignments\Homework01\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SourceData" sheetId="5" r:id="rId1"/>
@@ -688,39 +688,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -764,6 +731,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1082,7 +1082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1095,23 +1095,23 @@
       <c r="A1" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="48"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="42" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
       <c r="B4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="38" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       <c r="B5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="38" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
       <c r="B6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="38" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       <c r="B7" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       <c r="B8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="38" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       <c r="B9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="38" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       <c r="B10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="38" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1199,16 +1199,16 @@
       <c r="B11" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="39" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1236,47 +1236,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="54" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1296,7 +1296,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="55" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1342,7 +1342,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1360,7 +1360,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1378,7 +1378,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -1400,14 +1400,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1426,7 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1441,29 +1441,29 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="44" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="35" t="s">
@@ -1510,7 +1510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>37</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -1651,34 +1651,34 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1714,37 +1714,37 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="55" t="s">
+      <c r="G3" s="44" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="36" t="s">
@@ -1761,7 +1761,7 @@
       <c r="C4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="51" t="s">
         <v>83</v>
       </c>
       <c r="E4" s="18">
@@ -1787,7 +1787,7 @@
       <c r="C5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="51" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="18">
@@ -1813,7 +1813,7 @@
       <c r="C6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="51" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="18">
@@ -1839,7 +1839,7 @@
       <c r="C7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="52" t="s">
         <v>83</v>
       </c>
       <c r="E7" s="19">
@@ -1856,40 +1856,40 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1929,38 +1929,38 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="45" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="63"/>
       <c r="G3" s="29"/>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="47"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="63"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
@@ -1981,7 +1981,7 @@
       <c r="F4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="56"/>
+      <c r="G4" s="45"/>
       <c r="H4" s="11" t="s">
         <v>0</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="F5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="57"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="12" t="s">
         <v>19</v>
       </c>
@@ -2053,7 +2053,7 @@
       <c r="F6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="58"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="13" t="s">
         <v>20</v>
       </c>
@@ -2071,52 +2071,52 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>

</xml_diff>

<commit_message>
Completed paper for Homework01
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
@@ -191,9 +191,6 @@
     <t>Percent white population</t>
   </si>
   <si>
-    <t>Comparison of Univariate Global Spatial Autocorrelation of Select Regression Model Variables</t>
-  </si>
-  <si>
     <t>Bivariate Global Spatial Autocorrelation of Regression Model Variables Using Census Tracts Polygons</t>
   </si>
   <si>
@@ -337,6 +334,9 @@
   <si>
     <t>Grid Polygons 
 (1,000 meters X 1,000 meters)</t>
+  </si>
+  <si>
+    <t>Comparison of Univariate Global Spatial Autocorrelation Based on Census Tracts and Grid Polygons</t>
   </si>
 </sst>
 </file>
@@ -730,6 +730,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -762,9 +765,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1099,126 +1099,126 @@
   <sheetData>
     <row r="1" spans="1:3" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
+      <c r="A2" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="C4" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="C5" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="C6" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="C7" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="C8" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="C9" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="C10" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="C11" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="64" t="s">
-        <v>79</v>
+      <c r="A13" s="53" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1247,24 +1247,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
+      <c r="A1" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
@@ -1287,7 +1287,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="55" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1307,7 +1307,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="56" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1353,7 +1353,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1371,7 +1371,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1389,7 +1389,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -1411,14 +1411,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
+      <c r="A11" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1448,18 +1448,18 @@
   <sheetData>
     <row r="1" spans="1:6" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="A2" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
@@ -1498,7 +1498,7 @@
         <v>1E-3</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
         <v>1E-3</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1538,7 +1538,7 @@
         <v>1E-3</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>1E-3</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,7 +1578,7 @@
         <v>1E-3</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>1E-3</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
         <v>1E-3</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1638,7 +1638,7 @@
         <v>1E-3</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1658,38 +1658,38 @@
         <v>1E-3</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
+      <c r="A13" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
+      <c r="A14" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
+      <c r="A15" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1723,30 +1723,30 @@
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="A2" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="50" t="s">
         <v>44</v>
@@ -1775,7 +1775,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="18">
         <v>-0.248</v>
@@ -1787,7 +1787,7 @@
         <v>1E-3</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1813,7 +1813,7 @@
         <v>1E-3</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>1E-3</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1853,7 +1853,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="19">
         <v>0.248</v>
@@ -1865,44 +1865,44 @@
         <v>1E-3</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
+      <c r="A8" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
+      <c r="A9" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
+      <c r="A10" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1920,9 +1920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1940,42 +1938,42 @@
   <sheetData>
     <row r="1" spans="1:12" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
+      <c r="A2" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="48"/>
-      <c r="B3" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="63"/>
+      <c r="B3" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
       <c r="G3" s="29"/>
       <c r="H3" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="63"/>
+        <v>86</v>
+      </c>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="64"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
@@ -1992,7 +1990,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="45"/>
       <c r="H4" s="11" t="s">
@@ -2008,7 +2006,7 @@
         <v>14</v>
       </c>
       <c r="L4" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2028,7 +2026,7 @@
         <v>1E-3</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" s="46"/>
       <c r="H5" s="12" t="s">
@@ -2044,7 +2042,7 @@
         <v>1E-3</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2064,7 +2062,7 @@
         <v>1E-3</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="13" t="s">
@@ -2080,56 +2078,56 @@
         <v>1E-3</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
+      <c r="A7" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
+      <c r="A8" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
+      <c r="A9" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>

</xml_diff>

<commit_message>
Spatial regression with poverty and education
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SourceData" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
   <si>
     <t>Variable</t>
   </si>
@@ -337,6 +337,71 @@
   </si>
   <si>
     <t>Comparison of Univariate Global Spatial Autocorrelation Based on Census Tracts and Grid Polygons</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*** p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.001, ** p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.01, * p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.05</t>
+    </r>
+  </si>
+  <si>
+    <t>*** p ≤ 0.001, ** p ≤ 0.01, * p ≤ 0.05</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1152,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,15 +1500,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="6" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1483,16 +1552,16 @@
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C4" s="18">
-        <v>0.54</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="D4" s="16">
-        <v>9.4376999999999995</v>
+        <v>9.2829999999999995</v>
       </c>
       <c r="E4" s="14">
         <v>1E-3</v>
@@ -1503,16 +1572,16 @@
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C5" s="18">
-        <v>0.28499999999999998</v>
+        <v>0.54</v>
       </c>
       <c r="D5" s="16">
-        <v>5.0582000000000003</v>
+        <v>9.4376999999999995</v>
       </c>
       <c r="E5" s="14">
         <v>1E-3</v>
@@ -1523,16 +1592,16 @@
     </row>
     <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6" s="18">
-        <v>0.46</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="D6" s="16">
-        <v>7.9462000000000002</v>
+        <v>8.5184999999999995</v>
       </c>
       <c r="E6" s="14">
         <v>1E-3</v>
@@ -1603,16 +1672,16 @@
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="18">
-        <v>0.56899999999999995</v>
+        <v>0.46</v>
       </c>
       <c r="D10" s="16">
-        <v>9.2829999999999995</v>
+        <v>7.9462000000000002</v>
       </c>
       <c r="E10" s="14">
         <v>1E-3</v>
@@ -1623,16 +1692,16 @@
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="18">
-        <v>0.50800000000000001</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="D11" s="16">
-        <v>8.5184999999999995</v>
+        <v>5.3368000000000002</v>
       </c>
       <c r="E11" s="14">
         <v>1E-3</v>
@@ -1643,16 +1712,16 @@
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C12" s="19">
-        <v>0.29199999999999998</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D12" s="17">
-        <v>5.3368000000000002</v>
+        <v>5.0582000000000003</v>
       </c>
       <c r="E12" s="15">
         <v>1E-3</v>
@@ -1671,7 +1740,7 @@
       <c r="E13" s="58"/>
       <c r="F13" s="58"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
         <v>74</v>
       </c>
@@ -1683,7 +1752,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B15" s="60"/>
       <c r="C15" s="60"/>
@@ -1691,23 +1760,38 @@
       <c r="E15" s="60"/>
       <c r="F15" s="60"/>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <sortState ref="A4:F12">
+    <sortCondition descending="1" ref="C4:C12"/>
+  </sortState>
+  <mergeCells count="5">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A16:F16"/>
     <mergeCell ref="A15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,10 +1850,10 @@
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>18</v>
@@ -1778,10 +1862,10 @@
         <v>68</v>
       </c>
       <c r="E4" s="18">
-        <v>-0.248</v>
+        <v>0.248</v>
       </c>
       <c r="F4" s="16">
-        <v>-5.5247000000000002</v>
+        <v>5.7842000000000002</v>
       </c>
       <c r="G4" s="14">
         <v>1E-3</v>
@@ -1818,22 +1902,22 @@
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="E6" s="18">
-        <v>-0.499</v>
+        <v>-0.248</v>
       </c>
       <c r="F6" s="16">
-        <v>-9.1736000000000004</v>
+        <v>-5.5247000000000002</v>
       </c>
       <c r="G6" s="14">
         <v>1E-3</v>
@@ -1844,22 +1928,22 @@
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="E7" s="19">
-        <v>0.248</v>
+        <v>-0.499</v>
       </c>
       <c r="F7" s="17">
-        <v>5.7842000000000002</v>
+        <v>-9.1736000000000004</v>
       </c>
       <c r="G7" s="15">
         <v>1E-3</v>
@@ -1880,7 +1964,7 @@
       <c r="G8" s="58"/>
       <c r="H8" s="58"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>75</v>
       </c>
@@ -1894,7 +1978,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B10" s="60"/>
       <c r="C10" s="60"/>
@@ -1904,11 +1988,27 @@
       <c r="G10" s="60"/>
       <c r="H10" s="60"/>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <sortState ref="A4:H7">
+    <sortCondition descending="1" ref="E4:E7"/>
+  </sortState>
+  <mergeCells count="5">
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A11:H11"/>
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1918,9 +2018,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2011,16 +2113,16 @@
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="18">
-        <v>0.46500000000000002</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="D5" s="16">
-        <v>8.2940000000000005</v>
+        <v>8.0066000000000006</v>
       </c>
       <c r="E5" s="14">
         <v>1E-3</v>
@@ -2030,13 +2132,13 @@
       </c>
       <c r="G5" s="46"/>
       <c r="H5" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5" s="18">
-        <v>0.874</v>
+        <v>0.9</v>
       </c>
       <c r="J5" s="16">
-        <v>154.70519999999999</v>
+        <v>158.20840000000001</v>
       </c>
       <c r="K5" s="14">
         <v>1E-3</v>
@@ -2047,16 +2149,16 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="19">
-        <v>0.48599999999999999</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="D6" s="17">
-        <v>8.0066000000000006</v>
+        <v>8.2940000000000005</v>
       </c>
       <c r="E6" s="15">
         <v>1E-3</v>
@@ -2066,13 +2168,13 @@
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="19">
-        <v>0.9</v>
+        <v>0.874</v>
       </c>
       <c r="J6" s="17">
-        <v>158.20840000000001</v>
+        <v>154.70519999999999</v>
       </c>
       <c r="K6" s="15">
         <v>1E-3</v>
@@ -2097,7 +2199,7 @@
       <c r="K7" s="58"/>
       <c r="L7" s="58"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="61" t="s">
         <v>74</v>
       </c>
@@ -2115,7 +2217,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B9" s="61"/>
       <c r="C9" s="61"/>
@@ -2129,21 +2231,29 @@
       <c r="K9" s="61"/>
       <c r="L9" s="61"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="25"/>
@@ -2153,14 +2263,26 @@
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
     </row>
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <sortState ref="A5:L6">
+    <sortCondition descending="1" ref="C5:C6"/>
+  </sortState>
+  <mergeCells count="7">
     <mergeCell ref="A7:L7"/>
     <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A10:L10"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated legends for maps
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795"/>
   </bookViews>
   <sheets>
     <sheet name="SourceData" sheetId="5" r:id="rId1"/>
@@ -643,7 +643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -833,6 +833,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1151,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1300,7 +1303,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,13 +1361,13 @@
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="14">
         <v>476624.581427</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="14">
         <v>476939.12674899999</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="14">
         <v>473977.381995</v>
       </c>
       <c r="F4" s="30">
@@ -1376,13 +1379,13 @@
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="14">
         <v>4119126.7492479999</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="14">
         <v>4118697.1233649999</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="14">
         <v>4116847.817572</v>
       </c>
       <c r="F5" s="30">
@@ -1404,13 +1407,13 @@
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="66">
         <v>9.6719570000000008</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="66">
         <v>2.632361</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="66">
         <v>152.314719</v>
       </c>
       <c r="F7" s="30">
@@ -2020,7 +2023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added research question and hypotheses to presentation
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SourceData" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="88">
   <si>
     <t>Variable</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>Variable 2 Description</t>
-  </si>
-  <si>
-    <t>Percent white population</t>
   </si>
   <si>
     <t>Bivariate Global Spatial Autocorrelation of Regression Model Variables Using Census Tracts Polygons</t>
@@ -397,6 +394,9 @@
   <si>
     <t>Comparison of Univariate Global Spatial Autocorrelation 
 Based on Census Tracts and Grid Polygons</t>
+  </si>
+  <si>
+    <t>Percent White population</t>
   </si>
 </sst>
 </file>
@@ -1165,126 +1165,126 @@
   <sheetData>
     <row r="1" spans="1:3" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="C4" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="C5" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="C6" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="C7" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="C8" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="C9" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="C10" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="C11" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1314,7 +1314,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
@@ -1503,7 +1503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1517,12 +1517,12 @@
   <sheetData>
     <row r="1" spans="1:6" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
@@ -1565,7 +1565,7 @@
         <v>1E-3</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1585,7 +1585,7 @@
         <v>1E-3</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>1E-3</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>1E-3</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1645,7 +1645,7 @@
         <v>1E-3</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1665,7 +1665,7 @@
         <v>1E-3</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
         <v>1E-3</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1705,7 +1705,7 @@
         <v>1E-3</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1725,12 +1725,12 @@
         <v>1E-3</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="59"/>
       <c r="C13" s="59"/>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="61"/>
       <c r="C14" s="61"/>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="61"/>
       <c r="C16" s="61"/>
@@ -1786,10 +1786,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,12 +1806,12 @@
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
@@ -1823,13 +1823,13 @@
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="50" t="s">
         <v>43</v>
@@ -1847,147 +1847,175 @@
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="E4" s="18">
-        <v>0.248</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="F4" s="16">
-        <v>5.7842000000000002</v>
+        <v>-5.5247000000000002</v>
       </c>
       <c r="G4" s="14">
         <v>1E-3</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="E5" s="18">
-        <v>-0.21299999999999999</v>
+        <v>0.248</v>
       </c>
       <c r="F5" s="16">
-        <v>-4.7365000000000004</v>
+        <v>5.7842000000000002</v>
       </c>
       <c r="G5" s="14">
         <v>1E-3</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="E6" s="18">
-        <v>-0.248</v>
+        <v>-0.21299999999999999</v>
       </c>
       <c r="F6" s="16">
-        <v>-5.5247000000000002</v>
+        <v>-4.7365000000000004</v>
       </c>
       <c r="G6" s="14">
         <v>1E-3</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="18">
+        <v>-0.248</v>
+      </c>
+      <c r="F7" s="16">
+        <v>-5.5247000000000002</v>
+      </c>
+      <c r="G7" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="18">
+        <v>-0.42</v>
+      </c>
+      <c r="F8" s="16">
+        <v>-5.5247000000000002</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D9" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E9" s="19">
         <v>-0.499</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F9" s="17">
         <v>-9.1736000000000004</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G9" s="15">
         <v>1E-3</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="H9" s="24" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
@@ -1997,16 +2025,40 @@
       <c r="G11" s="61"/>
       <c r="H11" s="61"/>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+    </row>
   </sheetData>
-  <sortState ref="A4:H7">
-    <sortCondition descending="1" ref="E4:E7"/>
+  <sortState ref="A4:H9">
+    <sortCondition descending="1" ref="E4:E9"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2039,12 +2091,12 @@
   <sheetData>
     <row r="1" spans="1:12" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
@@ -2061,7 +2113,7 @@
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="48"/>
       <c r="B3" s="64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
@@ -2069,7 +2121,7 @@
       <c r="F3" s="66"/>
       <c r="G3" s="29"/>
       <c r="H3" s="67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I3" s="65"/>
       <c r="J3" s="65"/>
@@ -2123,7 +2175,7 @@
         <v>1E-3</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="46"/>
       <c r="H5" s="12" t="s">
@@ -2139,7 +2191,7 @@
         <v>1E-3</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2159,7 +2211,7 @@
         <v>1E-3</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="13" t="s">
@@ -2175,12 +2227,12 @@
         <v>1E-3</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -2196,7 +2248,7 @@
     </row>
     <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
@@ -2212,7 +2264,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="62"/>
       <c r="C9" s="62"/>
@@ -2228,7 +2280,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="62"/>
       <c r="C10" s="62"/>

</xml_diff>

<commit_message>
Reviewed numbering for tables and figures
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/docs/Townes_SOC5670_Homework01_Tables.xlsx
@@ -730,42 +730,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -814,6 +778,42 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1132,9 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1150,11 +1148,11 @@
       <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
@@ -1293,24 +1291,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -1333,7 +1331,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="63" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1353,7 +1351,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1379,7 +1377,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="64" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1399,7 +1397,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1417,7 +1415,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1433,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1457,14 +1455,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1499,13 +1497,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -1522,194 +1520,194 @@
       </c>
       <c r="E3" s="44"/>
     </row>
-    <row r="4" spans="1:5" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+    <row r="4" spans="1:5" s="49" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="46">
         <v>0.56899999999999995</v>
       </c>
-      <c r="C4" s="59">
+      <c r="C4" s="47">
         <v>9.2829999999999995</v>
       </c>
-      <c r="D4" s="60">
+      <c r="D4" s="48">
         <v>1E-3</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+    <row r="5" spans="1:5" s="49" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="46">
         <v>0.54</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="47">
         <v>9.4376999999999995</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="48">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+    <row r="6" spans="1:5" s="49" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="46">
         <v>0.50800000000000001</v>
       </c>
-      <c r="C6" s="59">
+      <c r="C6" s="47">
         <v>8.5184999999999995</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="48">
         <v>1E-3</v>
       </c>
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="61" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+    <row r="7" spans="1:5" s="49" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="46">
         <v>0.48599999999999999</v>
       </c>
-      <c r="C7" s="59">
+      <c r="C7" s="47">
         <v>8.3498999999999999</v>
       </c>
-      <c r="D7" s="60">
+      <c r="D7" s="48">
         <v>1E-3</v>
       </c>
-      <c r="E7" s="72" t="s">
+      <c r="E7" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+    <row r="8" spans="1:5" s="49" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="46">
         <v>0.48599999999999999</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="47">
         <v>8.0066000000000006</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="48">
         <v>1E-3</v>
       </c>
-      <c r="E8" s="72" t="s">
+      <c r="E8" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+    <row r="9" spans="1:5" s="49" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="58">
+      <c r="B9" s="46">
         <v>0.46500000000000002</v>
       </c>
-      <c r="C9" s="59">
+      <c r="C9" s="47">
         <v>8.2940000000000005</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="48">
         <v>1E-3</v>
       </c>
-      <c r="E9" s="72" t="s">
+      <c r="E9" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="61" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+    <row r="10" spans="1:5" s="49" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="46">
         <v>0.46</v>
       </c>
-      <c r="C10" s="59">
+      <c r="C10" s="47">
         <v>7.9462000000000002</v>
       </c>
-      <c r="D10" s="60">
+      <c r="D10" s="48">
         <v>1E-3</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+    <row r="11" spans="1:5" s="49" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="46">
         <v>0.29199999999999998</v>
       </c>
-      <c r="C11" s="59">
+      <c r="C11" s="47">
         <v>5.3368000000000002</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="48">
         <v>1E-3</v>
       </c>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="61" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
+    <row r="12" spans="1:5" s="49" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="63">
+      <c r="B12" s="51">
         <v>0.28499999999999998</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="52">
         <v>5.0582000000000003</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="53">
         <v>1E-3</v>
       </c>
-      <c r="E12" s="73" t="s">
+      <c r="E12" s="61" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
     </row>
     <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
     </row>
   </sheetData>
   <sortState ref="A4:F12">
@@ -1748,14 +1746,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -1791,7 +1789,7 @@
       <c r="E4" s="11">
         <v>1E-3</v>
       </c>
-      <c r="F4" s="69" t="s">
+      <c r="F4" s="57" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1811,7 +1809,7 @@
       <c r="E5" s="11">
         <v>1E-3</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="57" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1831,7 +1829,7 @@
       <c r="E6" s="11">
         <v>1E-3</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="57" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1851,7 +1849,7 @@
       <c r="E7" s="11">
         <v>1E-3</v>
       </c>
-      <c r="F7" s="69" t="s">
+      <c r="F7" s="57" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1871,7 +1869,7 @@
       <c r="E8" s="11">
         <v>1E-3</v>
       </c>
-      <c r="F8" s="69" t="s">
+      <c r="F8" s="57" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1891,49 +1889,49 @@
       <c r="E9" s="12">
         <v>1E-3</v>
       </c>
-      <c r="F9" s="70" t="s">
+      <c r="F9" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
     </row>
     <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
     </row>
   </sheetData>
   <sortState ref="A4:H9">
@@ -1979,41 +1977,41 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="53" t="s">
+      <c r="A3" s="54"/>
+      <c r="B3" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="56" t="s">
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
@@ -2040,7 +2038,7 @@
       <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="68"/>
+      <c r="L4" s="56"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
@@ -2074,7 +2072,7 @@
       <c r="K5" s="11">
         <v>1E-3</v>
       </c>
-      <c r="L5" s="69" t="s">
+      <c r="L5" s="57" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2110,73 +2108,73 @@
       <c r="K6" s="12">
         <v>1E-3</v>
       </c>
-      <c r="L6" s="70" t="s">
+      <c r="L6" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
     </row>
     <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="20"/>

</xml_diff>